<commit_message>
final plots and cluster names
</commit_message>
<xml_diff>
--- a/Clustering/clusters_profile.xlsx
+++ b/Clustering/clusters_profile.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos7\Desktop\Courses\Clustering\Final_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bill\Documents\GitHub\fall_3_orange_hw2\Clustering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E7E070-851C-4477-A14E-C79A91E699BB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D06D6D44-53D2-4515-92C7-129AAEC4239B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8424" xr2:uid="{6B95ECB5-F3C6-4E3B-BE0F-4B85C14321B7}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>SEQN</t>
   </si>
@@ -97,6 +97,42 @@
   </si>
   <si>
     <t>MCLUST:</t>
+  </si>
+  <si>
+    <t>Asthmatics</t>
+  </si>
+  <si>
+    <t>Lung Capacity</t>
+  </si>
+  <si>
+    <t>Monied Non-Smokers</t>
+  </si>
+  <si>
+    <t>Smoking, Not Asthmatic</t>
+  </si>
+  <si>
+    <t>Older Poorish People who are not asthmatic</t>
+  </si>
+  <si>
+    <t>Young poorish people</t>
+  </si>
+  <si>
+    <t>Just monied</t>
+  </si>
+  <si>
+    <t>x and y</t>
+  </si>
+  <si>
+    <t>x from k-means, y from mixture</t>
+  </si>
+  <si>
+    <t>1 and 6</t>
+  </si>
+  <si>
+    <t>3 and (4 or 5)</t>
+  </si>
+  <si>
+    <t>4 and 3 (maybe)</t>
   </si>
 </sst>
 </file>
@@ -530,27 +566,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{431A4ADB-8A85-4EB9-92C3-C56CD344B433}">
-  <dimension ref="C2:J69"/>
+  <dimension ref="B2:M69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.21875" customWidth="1"/>
+    <col min="3" max="3" width="15.5234375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.20703125" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.21875" customWidth="1"/>
-    <col min="9" max="10" width="10.109375" customWidth="1"/>
+    <col min="7" max="8" width="12.20703125" customWidth="1"/>
+    <col min="9" max="10" width="10.1015625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="C2" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="E4" t="s">
         <v>10</v>
       </c>
@@ -564,7 +600,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="C5" s="1"/>
       <c r="D5" t="s">
         <v>5</v>
@@ -582,7 +618,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
@@ -602,7 +638,7 @@
         <v>25658.92</v>
       </c>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
@@ -622,7 +658,7 @@
         <v>29.00779</v>
       </c>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
@@ -642,7 +678,7 @@
         <v>0.50283290000000003</v>
       </c>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
@@ -662,7 +698,7 @@
         <v>5.0991500000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="C10" s="1" t="s">
         <v>4</v>
       </c>
@@ -681,32 +717,57 @@
       <c r="H10" s="2">
         <v>2.1901030000000001</v>
       </c>
-    </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C11" s="1"/>
+      <c r="L10" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="E11" s="2">
+        <v>8.1300000000000008</v>
+      </c>
+      <c r="F11" s="2">
+        <v>5.47</v>
+      </c>
+      <c r="G11" s="2">
+        <v>5.77</v>
+      </c>
+      <c r="H11" s="2">
+        <v>7.86</v>
+      </c>
+      <c r="L11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="C12" s="1"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="L12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="C13" s="1"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="L13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="C14" s="1"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -714,7 +775,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.55000000000000004">
       <c r="C15" s="1"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -722,187 +783,217 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C16" s="5" t="s">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C18" s="4"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17" s="1"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" s="4"/>
+      <c r="C18" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="D18" s="2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="9" t="s">
+      <c r="G18" s="9" t="s">
         <v>17</v>
       </c>
+      <c r="H18" t="s">
+        <v>18</v>
+      </c>
       <c r="I18" t="s">
-        <v>18</v>
-      </c>
-      <c r="J18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C19" s="4" t="s">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="C19" s="2">
+        <v>27515.31</v>
+      </c>
       <c r="D19" s="2">
-        <v>27515.31</v>
+        <v>28703.45</v>
       </c>
       <c r="E19" s="2">
-        <v>28703.45</v>
+        <v>25725.33</v>
       </c>
       <c r="F19" s="2">
-        <v>25725.33</v>
-      </c>
-      <c r="G19" s="2">
         <v>27348.61</v>
       </c>
-      <c r="H19" s="7">
+      <c r="G19" s="7">
         <v>27725.63</v>
       </c>
+      <c r="H19" s="2">
+        <v>26837.98</v>
+      </c>
       <c r="I19" s="2">
-        <v>26837.98</v>
-      </c>
-      <c r="J19" s="2">
         <v>27920.82</v>
       </c>
     </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C20" s="4" t="s">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="C20" s="2">
+        <v>30.130299999999998</v>
+      </c>
       <c r="D20" s="2">
-        <v>30.130299999999998</v>
+        <v>30.039110000000001</v>
       </c>
       <c r="E20" s="2">
-        <v>30.039110000000001</v>
+        <v>30.64236</v>
       </c>
       <c r="F20" s="2">
-        <v>30.64236</v>
-      </c>
-      <c r="G20" s="2">
         <v>29.943290000000001</v>
       </c>
-      <c r="H20" s="7">
+      <c r="G20" s="7">
         <v>30.693490000000001</v>
       </c>
+      <c r="H20" s="2">
+        <v>29.523669999999999</v>
+      </c>
       <c r="I20" s="2">
-        <v>29.523669999999999</v>
-      </c>
-      <c r="J20" s="2">
         <v>30.44239</v>
       </c>
     </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C21" s="4" t="s">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="C21" s="2">
+        <v>0.4561249</v>
+      </c>
       <c r="D21" s="2">
-        <v>0.4561249</v>
+        <v>0.45018449999999999</v>
       </c>
       <c r="E21" s="2">
-        <v>0.45018449999999999</v>
+        <v>0.41935480000000003</v>
       </c>
       <c r="F21" s="2">
-        <v>0.41935480000000003</v>
-      </c>
-      <c r="G21" s="2">
         <v>0.47546349999999998</v>
       </c>
-      <c r="H21" s="7">
+      <c r="G21" s="7">
         <v>0.45210729999999999</v>
       </c>
+      <c r="H21" s="2">
+        <v>0.45956609999999998</v>
+      </c>
       <c r="I21" s="2">
-        <v>0.45956609999999998</v>
-      </c>
-      <c r="J21" s="2">
         <v>0.45420969999999999</v>
       </c>
     </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C22" s="4" t="s">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="C22" s="2">
+        <v>6.2573619999999996E-2</v>
+      </c>
       <c r="D22" s="2">
-        <v>6.2573619999999996E-2</v>
+        <v>0.10922510000000001</v>
       </c>
       <c r="E22" s="2">
-        <v>0.10922510000000001</v>
+        <v>4.9088359999999998E-2</v>
       </c>
       <c r="F22" s="2">
-        <v>4.9088359999999998E-2</v>
-      </c>
-      <c r="G22" s="2">
         <v>4.3075250000000002E-2</v>
       </c>
-      <c r="H22" s="7">
+      <c r="G22" s="7">
         <v>4.0229889999999997E-2</v>
       </c>
+      <c r="H22" s="2">
+        <v>4.9309659999999998E-2</v>
+      </c>
       <c r="I22" s="2">
-        <v>4.9309659999999998E-2</v>
-      </c>
-      <c r="J22" s="2">
         <v>6.7946820000000005E-2</v>
       </c>
     </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C23" s="4" t="s">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B23" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="C23" s="2">
+        <v>2.206534</v>
+      </c>
       <c r="D23" s="2">
-        <v>2.206534</v>
+        <v>2.1938970000000002</v>
       </c>
       <c r="E23" s="2">
-        <v>2.1938970000000002</v>
+        <v>2.4645229999999998</v>
       </c>
       <c r="F23" s="2">
-        <v>2.4645229999999998</v>
-      </c>
-      <c r="G23" s="2">
         <v>2.2226840000000001</v>
       </c>
-      <c r="H23" s="10">
+      <c r="G23" s="10">
         <v>1.7153179999999999</v>
       </c>
+      <c r="H23" s="2">
+        <v>1.800967</v>
+      </c>
       <c r="I23" s="2">
-        <v>1.800967</v>
-      </c>
-      <c r="J23" s="2">
         <v>2.5545520000000002</v>
       </c>
     </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B24" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="D24" s="2">
+        <v>5.75</v>
+      </c>
+      <c r="E24" s="2">
+        <v>7.61</v>
+      </c>
+      <c r="F24" s="2">
+        <v>7</v>
+      </c>
+      <c r="G24" s="2">
+        <v>5.7</v>
+      </c>
+      <c r="H24" s="2">
+        <v>6.06</v>
+      </c>
+      <c r="I24" s="2">
+        <v>7.51</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C25" s="1"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -910,7 +1001,7 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C26" s="1"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -918,7 +1009,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C27" s="1"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -926,7 +1017,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C28" s="1"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -934,7 +1025,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C29" s="1"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -942,7 +1033,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C30" s="1"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -950,7 +1041,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C31" s="1"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -958,7 +1049,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C32" s="1"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -966,7 +1057,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C33" s="1"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -974,7 +1065,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C34" s="1"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -982,7 +1073,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -990,7 +1081,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -998,7 +1089,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C37" s="1"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -1006,7 +1097,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -1014,7 +1105,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C39" s="1"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -1022,7 +1113,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C40" s="1"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -1030,7 +1121,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C41" s="1"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
@@ -1038,7 +1129,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C42" s="1"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -1046,7 +1137,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C43" s="1"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
@@ -1054,7 +1145,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C44" s="1"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -1062,7 +1153,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C45" s="1"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -1070,7 +1161,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C46" s="1"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -1078,7 +1169,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C47" s="1"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -1086,7 +1177,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C48" s="1"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -1094,7 +1185,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C49" s="1"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -1102,7 +1193,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C50" s="1"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -1110,7 +1201,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C51" s="1"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -1118,7 +1209,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C52" s="1"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -1126,7 +1217,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C53" s="1"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -1134,7 +1225,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C54" s="1"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -1142,7 +1233,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C55" s="1"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -1150,7 +1241,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C56" s="1"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
@@ -1158,7 +1249,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C57" s="1"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -1166,7 +1257,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C58" s="1"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -1174,7 +1265,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C59" s="1"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
@@ -1182,7 +1273,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C60" s="1"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -1190,7 +1281,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C61" s="1"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
@@ -1198,7 +1289,7 @@
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C62" s="1"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -1206,7 +1297,7 @@
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C63" s="1"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
@@ -1214,7 +1305,7 @@
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C64" s="1"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
@@ -1222,7 +1313,7 @@
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C65" s="1"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
@@ -1230,7 +1321,7 @@
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C66" s="1"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
@@ -1238,7 +1329,7 @@
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C67" s="1"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
@@ -1246,7 +1337,7 @@
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C68" s="1"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
@@ -1254,7 +1345,7 @@
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C69" s="1"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>

</xml_diff>